<commit_message>
added an option to save images
</commit_message>
<xml_diff>
--- a/examples/example_widedata.xlsx
+++ b/examples/example_widedata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenelkayam/flamholz_lab/wf_trial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edenelkayam/flamholz_lab/wellflow/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA170E61-430E-F641-822B-17F97408CA64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDA73B7-CB26-F749-8594-A8F58A700118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="1000" windowWidth="24820" windowHeight="14060" xr2:uid="{86BAC9DE-1231-4545-80D2-4A0BBE0DFAE8}"/>
   </bookViews>
@@ -613,8 +613,8 @@
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>673484</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -646,8 +646,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2316480" y="5379720"/>
-          <a:ext cx="594360" cy="152400"/>
+          <a:off x="2584104" y="5268422"/>
+          <a:ext cx="658244" cy="157942"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6879,8 +6879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82400A6-3200-40EA-A3B6-A1D7E10792B7}">
   <dimension ref="A2:CU285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A244" sqref="A244"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>